<commit_message>
Cambios finales de subir excel
</commit_message>
<xml_diff>
--- a/public/excels/ejemploExcelMinimoMaximo.xlsx
+++ b/public/excels/ejemploExcelMinimoMaximo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Milly\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A1547A5F-BA80-41A9-9340-9B3212F151A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A8547B3-9699-421F-AD11-1BDCF557FD4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{8E123716-2BA3-4AD7-81A9-6B1EB89D2983}"/>
   </bookViews>
@@ -391,7 +391,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -412,10 +412,10 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C2">
-        <v>4</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>